<commit_message>
Melhorias organizacionais no código e pastas
Também retirados os comentários na planilha
</commit_message>
<xml_diff>
--- a/planilha_mapeamento_v3.xlsx
+++ b/planilha_mapeamento_v3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\_Programming\template-builder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frost\Meu Drive\_Programming\template-builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64253602-D9E6-4E61-B072-ED69D3E0D6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0EB5487-0F5A-497F-BEA2-5138DB9F0F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F5624AC8-C326-4C6C-9A77-0DDF267B8F11}"/>
   </bookViews>
@@ -37,213 +37,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={BA108348-5E3A-4F5F-A9E0-F181EF87A340}</author>
-    <author>tc={79050BAE-2F9F-4E1D-9A90-23184430FFEF}</author>
-    <author>tc={2FC44181-20F6-4267-AEE4-8ED35D3A50B1}</author>
-    <author>tc={5B517CE5-1116-490C-9A52-3D06B5B0ECA9}</author>
-    <author>tc={0C7CF347-E2DD-401A-B736-723FC203500B}</author>
-    <author>tc={F48B872B-A719-4F3E-81DC-1ADF666FB740}</author>
-    <author>tc={2C3CD18C-EDFB-44EE-8856-5E40FF94A083}</author>
-    <author>tc={41F5E509-625C-43D5-A01B-CD7914B4F056}</author>
-    <author>tc={9A8D7C1D-04FF-4F82-BF10-F61473D8A4AB}</author>
-    <author>tc={A9693B07-4846-443B-82AC-C82AE76B1532}</author>
-    <author>tc={8910DEDA-FB31-4FA8-AF83-B41DE03CBB76}</author>
-    <author>tc={B6C1D987-EAB5-4DCC-AA5B-34F0EC804D0B}</author>
-    <author>tc={AF237C9F-15E9-43FB-A33C-32130B2ECC0A}</author>
-    <author>tc={B2BF9114-BF3C-4321-9F38-6B204D8DF8D6}</author>
-    <author>tc={B3F8982A-F27A-423D-AA0A-EEEA4F1098FC}</author>
-    <author>tc={F3CEB59B-A42E-4625-824F-D415D268E468}</author>
-    <author>tc={A5915FD8-E091-4A55-AEDA-E9F4C637D9EE}</author>
-    <author>tc={6382AB26-25D1-4B63-B0FA-252773452608}</author>
-    <author>tc={7743B299-32EB-4A81-9A8F-1B27F87F8660}</author>
-    <author>tc={9FED2ED9-4709-4031-9E9E-6211B6E2326E}</author>
-    <author>tc={85717179-FF48-4904-92E1-C4C7EA1B9676}</author>
-    <author>tc={35B1D935-276D-4F0A-B141-9BE4E4FE035B}</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{BA108348-5E3A-4F5F-A9E0-F181EF87A340}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    O código do ponto de campo. Ex: PTI-2001. Não deixe em branco. Preencha na ordem de numeração. Não repita nenhum código já inserido em linhas subsequentes.</t>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="1" shapeId="0" xr:uid="{79050BAE-2F9F-4E1D-9A90-23184430FFEF}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    A numeração ou identificação da subárea mapeada pelo grupo.</t>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="2" shapeId="0" xr:uid="{2FC44181-20F6-4267-AEE4-8ED35D3A50B1}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    A fase ou disciplina de mapeamento na qual o ponto foi visitado pela primeira vez. Não deixe em branco. Ex: "Mapeamento Geológico I". Preencha apenas de forma contínua (depois que preencher uma linha com “Mapeamento Geológico II”, por exemplo, não preencha nenhuma linha seguinte com “Mapeamento Geológico I”).</t>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="3" shapeId="0" xr:uid="{5B517CE5-1116-490C-9A52-3D06B5B0ECA9}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    O sistema de referência de coordenadas utilizado. Ex: "WGS 84 / UTM zone 22S". Não deixe em branco.</t>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="4" shapeId="0" xr:uid="{0C7CF347-E2DD-401A-B736-723FC203500B}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    A coordenada UTM leste (easting) do ponto, em metros. Insira apenas números. Não deixe em branco.</t>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="5" shapeId="0" xr:uid="{F48B872B-A719-4F3E-81DC-1ADF666FB740}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    A coordenada UTM norte (northing) do ponto, em metros. Insira apenas números. Não deixe em branco.</t>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="6" shapeId="0" xr:uid="{2C3CD18C-EDFB-44EE-8856-5E40FF94A083}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    A altitude do ponto, em metros. Insira apenas números.</t>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="7" shapeId="0" xr:uid="{41F5E509-625C-43D5-A01B-CD7914B4F056}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    A sigla do estado onde o ponto está localizado. Não deixe em branco.</t>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="8" shapeId="0" xr:uid="{9A8D7C1D-04FF-4F82-BF10-F61473D8A4AB}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    O município no qual o ponto está inserido.</t>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="9" shapeId="0" xr:uid="{A9693B07-4846-443B-82AC-C82AE76B1532}">
-      <text>
-        <t xml:space="preserve">[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    A toponímia do local ou um local de referência próximo ao ponto. Utilize apenas referências duradouras e que possam ajudar alguém que nunca esteve no local a encontrar o ponto no futuro. </t>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="10" shapeId="0" xr:uid="{8910DEDA-FB31-4FA8-AF83-B41DE03CBB76}">
-      <text>
-        <t xml:space="preserve">[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    A data em que o ponto foi visitado pela primeira vez, no formato dia/mês/ano. Ex: "01/08/1997". Não deixe em branco. </t>
-      </text>
-    </comment>
-    <comment ref="L1" authorId="11" shapeId="0" xr:uid="{B6C1D987-EAB5-4DCC-AA5B-34F0EC804D0B}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    Os nomes dos integrantes da equipe que visitou o ponto, incluindo professores, separados por vírgula e espaço. Utilize apenas o último sobrenome de cada integrante, e nenhum nome do meio. Ex: "Ana Sutili, Gabriel Maccari, Vicente Wetter, Luana Florisbal". Não deixe em branco.</t>
-      </text>
-    </comment>
-    <comment ref="M1" authorId="12" shapeId="0" xr:uid="{AF237C9F-15E9-43FB-A33C-32130B2ECC0A}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    Se o ponto em questão é apenas um ponto de controle, ou se possui afloramento. Preencha com “Sim” ou “Não” (sem aspas, com acento, inicial maiúscula). Não deixe em branco. Se o ponto possui afloramento e foi possível determinar a litologia, preencha com "Não".</t>
-      </text>
-    </comment>
-    <comment ref="N1" authorId="13" shapeId="0" xr:uid="{B2BF9114-BF3C-4321-9F38-6B204D8DF8D6}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    O número de amostras coletadas no ponto. Preencha apenas com números inteiros. Preencha com zero caso nenhuma amostra tenha sido coletada. Não deixe em branco.</t>
-      </text>
-    </comment>
-    <comment ref="O1" authorId="14" shapeId="0" xr:uid="{B3F8982A-F27A-423D-AA0A-EEEA4F1098FC}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    Se foram feitas lâminas petrográficas a partir das amostras coletadas no ponto. Preencha com "Sim" ou "Não" (sem aspas, com acento, inicial maiúscula). Não deixe em branco.</t>
-      </text>
-    </comment>
-    <comment ref="P1" authorId="15" shapeId="0" xr:uid="{F3CEB59B-A42E-4625-824F-D415D268E468}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    O tipo de afloramento presente no ponto em questão. Ex: "Corte de estrada", "Barranco", "Drenagem", etc. Deixe em branco apenas nos pontos de controle.</t>
-      </text>
-    </comment>
-    <comment ref="Q1" authorId="16" shapeId="0" xr:uid="{A5915FD8-E091-4A55-AEDA-E9F4C637D9EE}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    Se as rochas descritas no ponto encontravam-se in situ ou se foram transportadas de outro local (como no caso de matacões rolados morro abaixo). Preencha com “Sim” ou “Não” (sem aspas, com acento, inicial maiúscula). No caso de depósitos sedimentares inconsolidados, preencha sempre com "Sim". Deixe em branco apenas nos pontos de controle.</t>
-      </text>
-    </comment>
-    <comment ref="R1" authorId="17" shapeId="0" xr:uid="{6382AB26-25D1-4B63-B0FA-252773452608}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    O grau de alteração do afloramento frente às intempéries. Preencha com “Baixo”, “Médio” ou “Alto” (sem aspas, com acento, inicial maiúscula). Deixe em branco apenas nos pontos de controle.</t>
-      </text>
-    </comment>
-    <comment ref="S1" authorId="18" shapeId="0" xr:uid="{7743B299-32EB-4A81-9A8F-1B27F87F8660}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    A unidade maior na qual a litologia principal do ponto está contida. O preenchimento deste campo deve ser feito conforme as unidades listadas na segunda aba da planilha. Ex: "Complexo Metamórfico Brusque", "Suíte Valsungana", "Coberturas Cenozoicas", etc. Deixe em branco apenas nos pontos de controle.</t>
-      </text>
-    </comment>
-    <comment ref="T1" authorId="19" shapeId="0" xr:uid="{9FED2ED9-4709-4031-9E9E-6211B6E2326E}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    A unidade litoestratigráfica específica na qual a litologia principal do ponto está contida. O preenchimento deste campo deve ser feito conforme as unidades litoestratigráficas listadas na segunda aba da planilha. Ex: "Formação Rio Bonito", "Granodiorito Estaleiro", etc. Deixe em branco apenas nos pontos de controle.</t>
-      </text>
-    </comment>
-    <comment ref="U1" authorId="20" shapeId="0" xr:uid="{85717179-FF48-4904-92E1-C4C7EA1B9676}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    A unidade maior na qual a litologia secundária do ponto está contida. O preenchimento deste campo deve ser feito conforme as unidades listadas na segunda aba da planilha. Preencha apenas caso o afloramento apresente contato entre duas unidades distintas. Não preencha nos pontos de controle.</t>
-      </text>
-    </comment>
-    <comment ref="V1" authorId="21" shapeId="0" xr:uid="{35B1D935-276D-4F0A-B141-9BE4E4FE035B}">
-      <text>
-        <t>[Comentário encadeado]
-Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
-Comentário:
-    A unidade litoestratigráfica específica na qual a litologia secundária do ponto está contida. O preenchimento deste campo deve ser feito conforme as unidades litoestratigráficas listadas na segunda aba da planilha. Preencha apenas caso o afloramento apresente contato entre duas unidades distintas. Não preencha nos pontos de controle.</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1280,22 +1073,22 @@
     <text>O grau de alteração do afloramento frente às intempéries. Preencha com “Baixo”, “Médio” ou “Alto” (sem aspas, com acento, inicial maiúscula). Deixe em branco apenas nos pontos de controle.</text>
   </threadedComment>
   <threadedComment ref="S1" dT="2024-10-18T20:43:39.49" personId="{98F0DC76-0982-41DC-B8C5-8118CFBE9B66}" id="{7743B299-32EB-4A81-9A8F-1B27F87F8660}">
-    <text>A unidade maior na qual a litologia principal do ponto está contida. O preenchimento deste campo deve ser feito conforme as unidades listadas na segunda aba da planilha. Ex: "Complexo Metamórfico Brusque", "Suíte Valsungana", "Coberturas Cenozoicas", etc. Deixe em branco apenas nos pontos de controle.</text>
+    <text>A unidade maior na qual a litologia principal do ponto está contida. O preenchimento deste campo deve ser feito conforme as unidades listadas aba Listas da planilha. Ex: "Complexo Metamórfico Brusque", "Suíte Valsungana", "Coberturas Cenozoicas", etc. Deixe em branco apenas nos pontos de controle.</text>
   </threadedComment>
   <threadedComment ref="T1" dT="2024-10-18T20:44:24.01" personId="{98F0DC76-0982-41DC-B8C5-8118CFBE9B66}" id="{9FED2ED9-4709-4031-9E9E-6211B6E2326E}">
-    <text>A unidade litoestratigráfica específica na qual a litologia principal do ponto está contida. O preenchimento deste campo deve ser feito conforme as unidades litoestratigráficas listadas na segunda aba da planilha. Ex: "Formação Rio Bonito", "Granodiorito Estaleiro", etc. Deixe em branco apenas nos pontos de controle.</text>
+    <text>A unidade litoestratigráfica específica na qual a litologia principal do ponto está contida. O preenchimento deste campo deve ser feito conforme as unidades litoestratigráficas listadas na aba Listas da planilha. Ex: "Formação Rio Bonito", "Granodiorito Estaleiro", etc. Deixe em branco apenas nos pontos de controle.</text>
   </threadedComment>
   <threadedComment ref="U1" dT="2024-10-18T20:45:21.31" personId="{98F0DC76-0982-41DC-B8C5-8118CFBE9B66}" id="{85717179-FF48-4904-92E1-C4C7EA1B9676}">
-    <text>A unidade maior na qual a litologia secundária do ponto está contida. O preenchimento deste campo deve ser feito conforme as unidades listadas na segunda aba da planilha. Preencha apenas caso o afloramento apresente contato entre duas unidades distintas. Não preencha nos pontos de controle.</text>
+    <text>A unidade maior na qual a litologia secundária do ponto está contida. O preenchimento deste campo deve ser feito conforme as unidades listadas na aba Listas da planilha. Preencha apenas caso o afloramento apresente contato entre duas unidades distintas. Não preencha nos pontos de controle.</text>
   </threadedComment>
   <threadedComment ref="V1" dT="2024-10-18T20:45:53.04" personId="{98F0DC76-0982-41DC-B8C5-8118CFBE9B66}" id="{35B1D935-276D-4F0A-B141-9BE4E4FE035B}">
-    <text>A unidade litoestratigráfica específica na qual a litologia secundária do ponto está contida. O preenchimento deste campo deve ser feito conforme as unidades litoestratigráficas listadas na segunda aba da planilha. Preencha apenas caso o afloramento apresente contato entre duas unidades distintas. Não preencha nos pontos de controle.</text>
+    <text>A unidade litoestratigráfica específica na qual a litologia secundária do ponto está contida. O preenchimento deste campo deve ser feito conforme as unidades litoestratigráficas listadas na aba Listas da planilha. Preencha apenas caso o afloramento apresente contato entre duas unidades distintas. Não preencha nos pontos de controle.</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD92E1D2-10EB-4B21-AC3E-CAB6F478E8EB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD92E1D2-10EB-4B21-AC3E-CAB6F478E8EB}">
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1397,7 +1190,7 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertHyperlinks="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <dataValidations count="13">
+  <dataValidations count="12">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dado inválido" error="Insira uma coordenada UTM (easting) válida." sqref="E2:E1048576" xr:uid="{7C59531C-1D22-4B31-B4C7-5F3CE27BAA76}">
       <formula1>165000</formula1>
       <formula2>835000</formula2>
@@ -1413,14 +1206,11 @@
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dado inválido" error="Insira uma data válida (dd/mm/aaaa)." sqref="K2:K1048576" xr:uid="{CD0A578C-71A8-4A96-84F8-735E01EC6E06}">
       <formula1>18264</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dado inválido" error="Insira &quot;Sim&quot; ou &quot;Não&quot; (sem aspas)." sqref="O2:O1048576 M2:M1048576" xr:uid="{04721667-D8B1-45D0-BD9F-4AECA3B5AF11}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dado inválido" error="Insira &quot;Sim&quot; ou &quot;Não&quot; (sem aspas)." sqref="O2:O1048576 M2:M1048576 Q2:Q1048576" xr:uid="{04721667-D8B1-45D0-BD9F-4AECA3B5AF11}">
       <formula1>"Sim,Não"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dado inválido" error="Insira &quot;Baixo&quot;, &quot;Médio&quot; ou &quot;Alto&quot; (sem aspas). Deixe em branco caso seja um ponto de controle." sqref="R2:R1048576" xr:uid="{2A9DAFDA-2615-4A94-B3D1-168A60EDA4C3}">
       <formula1>"Baixo,Médio,Alto"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dado inválido" error="Insira &quot;Sim&quot; ou &quot;Não&quot; (sem aspas)." sqref="Q2:Q1048576" xr:uid="{62FC924A-79E9-48FD-B7DA-0276C7FAA1AE}">
-      <formula1>"Sim,Não"</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dado inválido" error="Insira o número de amostras coletadas no ponto. Preencha com zero caso não haja amostras." sqref="N2:N1048576" xr:uid="{CBCA314D-06D8-40E2-AED0-028E53FAC418}">
       <formula1>0</formula1>
@@ -1444,10 +1234,9 @@
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dado inválido" error="Preencha com uma das opções da lista de faixas/áreas do projeto." xr:uid="{0AD58989-B90C-41FD-B6EA-76E5FA7ABF6D}">
           <x14:formula1>
             <xm:f>Listas!$E$2:$E$31</xm:f>
@@ -1464,25 +1253,13 @@
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$31</xm:f>
           </x14:formula1>
-          <xm:sqref>U2:U1048576</xm:sqref>
+          <xm:sqref>U2:U1048576 S2:S1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dado inválido" error="Preencha com uma das opções da lista de unidades litoestratigráficas." xr:uid="{8683B692-9403-4B82-9F23-F93E5A70F048}">
           <x14:formula1>
             <xm:f>Listas!$B$2:$B$31</xm:f>
           </x14:formula1>
-          <xm:sqref>V2:V1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dado inválido" error="Preencha com uma das opções da lista de unidades litoestratigráficas." xr:uid="{ADEEBC44-3A49-4C22-8EF2-D9A2861E5136}">
-          <x14:formula1>
-            <xm:f>Listas!$B$2:$B$31</xm:f>
-          </x14:formula1>
-          <xm:sqref>T2:T1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dado inválido" error="Preencha com uma das opções da lista de unidades geológicas." xr:uid="{181772FC-BC76-452A-A47F-B73D99C84F65}">
-          <x14:formula1>
-            <xm:f>Listas!$A$2:$A$31</xm:f>
-          </x14:formula1>
-          <xm:sqref>S2:S1048576</xm:sqref>
+          <xm:sqref>V2:V1048576 T2:T1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1495,7 +1272,7 @@
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2299,7 +2076,7 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>